<commit_message>
Standardized names for repos
</commit_message>
<xml_diff>
--- a/8001/ACTUALS@latest/Operator Reports/DevOps/Repo Stats.xlsx
+++ b/8001/ACTUALS@latest/Operator Reports/DevOps/Repo Stats.xlsx
@@ -8,23 +8,23 @@
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
-    <sheet name="foo_app (Local)" sheetId="2" r:id="rId2"/>
-    <sheet name="foo_app (Remote)" sheetId="3" r:id="rId3"/>
-    <sheet name="foo_app_docs (Local)" sheetId="4" r:id="rId4"/>
-    <sheet name="foo_app_docs (Remote)" sheetId="5" r:id="rId5"/>
-    <sheet name="foo_app_test (Local)" sheetId="6" r:id="rId6"/>
-    <sheet name="foo_app_test (Remote)" sheetId="7" r:id="rId7"/>
-    <sheet name="foo_app_scenarios (Local)" sheetId="8" r:id="rId8"/>
-    <sheet name="foo_app_scenarios (Remote)" sheetId="9" r:id="rId9"/>
-    <sheet name="foo_app_ops (Local)" sheetId="10" r:id="rId10"/>
-    <sheet name="foo_app_ops (Remote)" sheetId="11" r:id="rId11"/>
+    <sheet name="foo_app.svc (Local)" sheetId="2" r:id="rId2"/>
+    <sheet name="foo_app.svc (Remote)" sheetId="3" r:id="rId3"/>
+    <sheet name="foo_app.docs (Local)" sheetId="4" r:id="rId4"/>
+    <sheet name="foo_app.docs (Remote)" sheetId="5" r:id="rId5"/>
+    <sheet name="foo_app.test (Local)" sheetId="6" r:id="rId6"/>
+    <sheet name="foo_app.test (Remote)" sheetId="7" r:id="rId7"/>
+    <sheet name="foo_app.scenarios (Local)" sheetId="8" r:id="rId8"/>
+    <sheet name="foo_app.scenarios (Remote)" sheetId="9" r:id="rId9"/>
+    <sheet name="foo_app.ops (Local)" sheetId="10" r:id="rId10"/>
+    <sheet name="foo_app.ops (Remote)" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="29">
   <si>
     <t>Repo</t>
   </si>
@@ -35,12 +35,15 @@
     <t>Current Branch</t>
   </si>
   <si>
-    <t>Is dirty</t>
-  </si>
-  <si>
     <t># Untracked files</t>
   </si>
   <si>
+    <t># Modified files</t>
+  </si>
+  <si>
+    <t># Deleted files</t>
+  </si>
+  <si>
     <t>Last commit</t>
   </si>
   <si>
@@ -50,7 +53,7 @@
     <t>Last commit hash</t>
   </si>
   <si>
-    <t>foo_app</t>
+    <t>foo_app.svc</t>
   </si>
   <si>
     <t>Local</t>
@@ -71,16 +74,16 @@
     <t>master</t>
   </si>
   <si>
-    <t>foo_app_docs</t>
-  </si>
-  <si>
-    <t>foo_app_test</t>
-  </si>
-  <si>
-    <t>foo_app_scenarios</t>
-  </si>
-  <si>
-    <t>foo_app_ops</t>
+    <t>foo_app.docs</t>
+  </si>
+  <si>
+    <t>foo_app.test</t>
+  </si>
+  <si>
+    <t>foo_app.scenarios</t>
+  </si>
+  <si>
+    <t>foo_app.ops</t>
   </si>
   <si>
     <t>Commit #</t>
@@ -105,9 +108,6 @@
   </si>
   <si>
     <t>.gitignore</t>
-  </si>
-  <si>
-    <t>Alejandro Hernandez &lt;alejandro.hernandez@finastra.com&gt;</t>
   </si>
   <si>
     <t>README.md</t>
@@ -486,7 +486,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -502,12 +502,13 @@
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="40.7109375" customWidth="1"/>
-    <col min="7" max="7" width="30.7109375" customWidth="1"/>
-    <col min="8" max="8" width="45.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="40.7109375" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" customWidth="1"/>
+    <col min="9" max="9" width="45.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -532,265 +533,298 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="C5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="2" t="s">
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="3" t="s">
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="C11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="3" t="b">
+        <v>15</v>
+      </c>
+      <c r="D11" s="3">
         <v>0</v>
       </c>
       <c r="E11" s="3">
         <v>0</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>11</v>
+      <c r="F11" s="3">
+        <v>0</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -822,25 +856,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -848,22 +882,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -871,10 +905,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
@@ -883,10 +917,10 @@
         <v>28</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -918,25 +952,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -944,22 +978,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -967,10 +1001,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
@@ -979,10 +1013,10 @@
         <v>28</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1014,25 +1048,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1040,22 +1074,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1063,10 +1097,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
@@ -1075,10 +1109,10 @@
         <v>28</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1110,25 +1144,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1136,22 +1170,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1159,10 +1193,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
@@ -1171,10 +1205,10 @@
         <v>28</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1206,25 +1240,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1232,22 +1266,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1255,10 +1289,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
@@ -1267,10 +1301,10 @@
         <v>28</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1302,25 +1336,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1328,22 +1362,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1351,10 +1385,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
@@ -1363,10 +1397,10 @@
         <v>28</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1398,25 +1432,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1424,22 +1458,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1447,10 +1481,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
@@ -1459,10 +1493,10 @@
         <v>28</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1494,25 +1528,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1520,22 +1554,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1543,10 +1577,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
@@ -1555,10 +1589,10 @@
         <v>28</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1590,25 +1624,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1616,22 +1650,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1639,10 +1673,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
@@ -1651,10 +1685,10 @@
         <v>28</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1686,25 +1720,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1712,22 +1746,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1735,10 +1769,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
@@ -1747,10 +1781,10 @@
         <v>28</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>